<commit_message>
Somewhat fixed the sounds for the finish line system
</commit_message>
<xml_diff>
--- a/Logbook Ruben Flinterman.xlsx
+++ b/Logbook Ruben Flinterman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwfli\Documents\1. Studie\INF\Challengeweeks\Challengeweek 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9245E2F-E6A8-4E86-A87A-F529B503CAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA0F513-D0E3-4E16-8214-C0E7CD62266C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Drop down items" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>🤔 Why keep a logbook?</t>
   </si>
@@ -333,16 +332,29 @@
   <si>
     <t>Added some items and images</t>
   </si>
+  <si>
+    <t>Added finish line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding the finish line took some time as I needed to chane both the code and the map. I also added sound for each finished lap and when you actually finish. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -451,45 +463,51 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="46" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="46" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2245,7 +2263,7 @@
   <dimension ref="B1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2301,7 +2319,7 @@
       </c>
       <c r="F4" s="15">
         <f>SUM(D4:D97)</f>
-        <v>1.645833333333333</v>
+        <v>1.770833333333333</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.2">
@@ -2640,11 +2658,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="12"/>
+    <row r="29" spans="2:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="B29" s="12">
+        <v>45261</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="14">
+        <v>0.125</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="30" spans="2:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="12"/>
@@ -5693,15 +5719,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ABCCEE9817AF674CAD101E6D861B9A46" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="946de471897b9ab3b9496c906eacb5e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40058f32-786b-4391-91be-af0d896640a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a00be7a65770b509424fc2b063afb2cd" ns2:_="">
     <xsd:import namespace="40058f32-786b-4391-91be-af0d896640a5"/>
@@ -5839,6 +5856,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5846,14 +5872,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78E03D4F-D06B-40C1-A53D-F1DEB199C8A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4BE0F66-9181-4FFE-AE37-08F456A06E70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5871,6 +5889,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78E03D4F-D06B-40C1-A53D-F1DEB199C8A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14BB4D6E-C856-4503-A5F5-487F247D347A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added player 2, position not yet seperated from player 1
</commit_message>
<xml_diff>
--- a/Logbook Ruben Flinterman.xlsx
+++ b/Logbook Ruben Flinterman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwfli\Documents\1. Studie\INF\Challengeweeks\Challengeweek 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF349080-BCC5-4E08-853A-E90C4B760AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FEC962-76BC-4736-9DA9-9AADA59BE129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
   <si>
     <t>🤔 Why keep a logbook?</t>
   </si>
@@ -338,16 +338,29 @@
   <si>
     <t xml:space="preserve">Adding the finish line took some time as I needed to chane both the code and the map. I also added and fixed each sound for each finished lap and for when you actually finish. </t>
   </si>
+  <si>
+    <t>Did research on AI with pygame and tested example code.</t>
+  </si>
+  <si>
+    <t>Researched and played with AI so we can make a player 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -470,51 +483,54 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="46" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="46" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -991,6 +1007,94 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1800225</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>2572</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E1D3B99-94F8-1F6B-0C43-747B75A329AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11430000" y="11449049"/>
+          <a:ext cx="2790825" cy="2079023"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1800225</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>7365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>390114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07584687-0AE9-C75C-C03C-A85EBE528DE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14220825" y="11446890"/>
+          <a:ext cx="2790825" cy="2078199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2270,7 +2374,7 @@
   <dimension ref="B1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2326,7 +2430,7 @@
       </c>
       <c r="F4" s="15">
         <f>SUM(D4:D97)</f>
-        <v>1.8124999999999998</v>
+        <v>1.9374999999999998</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.2">
@@ -2680,10 +2784,18 @@
       </c>
     </row>
     <row r="30" spans="2:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="13"/>
+      <c r="B30" s="12">
+        <v>45261</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="14">
+        <v>0.125</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="31" spans="2:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="12"/>
@@ -5726,15 +5838,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ABCCEE9817AF674CAD101E6D861B9A46" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="946de471897b9ab3b9496c906eacb5e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40058f32-786b-4391-91be-af0d896640a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a00be7a65770b509424fc2b063afb2cd" ns2:_="">
     <xsd:import namespace="40058f32-786b-4391-91be-af0d896640a5"/>
@@ -5872,6 +5975,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5879,14 +5991,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78E03D4F-D06B-40C1-A53D-F1DEB199C8A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4BE0F66-9181-4FFE-AE37-08F456A06E70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5904,6 +6008,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78E03D4F-D06B-40C1-A53D-F1DEB199C8A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14BB4D6E-C856-4503-A5F5-487F247D347A}">
   <ds:schemaRefs>

</xml_diff>